<commit_message>
data extraction for acclimation set and screening file for scopus search
</commit_message>
<xml_diff>
--- a/data extraction /fullvariability_7jun21.xlsx
+++ b/data extraction /fullvariability_7jun21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F35013-E44E-814E-926D-5ADC1E62E048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDFBD11-CF52-FE44-84CA-B48F5C49D002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-13240" windowWidth="24800" windowHeight="15160" xr2:uid="{1590338E-647F-824F-9766-668D1776E023}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="269">
   <si>
     <t>label</t>
   </si>
@@ -808,6 +808,30 @@
   </si>
   <si>
     <t>microbiota in sludge, it seems like they have a paired set of experiments but unclear…</t>
+  </si>
+  <si>
+    <t>Bernhardt_2018_PROFTHROSOB.SC</t>
+  </si>
+  <si>
+    <t>Bernhardt, Joey R. and Sunday, Jennifer M. and Thompson, Patrick L. and O'Connor, Mary I.</t>
+  </si>
+  <si>
+    <t>Nonlinear averaging of thermal experience predicts population growth rates in a thermally variable environment</t>
+  </si>
+  <si>
+    <t>PROCEEDINGS OF THE ROYAL SOCIETY B-BIOLOGICAL SCIENCES</t>
+  </si>
+  <si>
+    <t>10.1098/rspb.2018.1076</t>
+  </si>
+  <si>
+    <t>As thermal regimes change worldwide, projections of future population and species persistence often require estimates of how population growth rates depend on temperature. These projections rarely account for how temporal variation in temperature can systematically modify growth rates relative to projections based on constant temperatures. Here, we tested the hypothesis that time-averaged population growth rates in fluctuating thermal environments differ from growth rates in constant conditions as a consequence of Jensen's inequality, and that the thermal performance curves (TPCs) describing population growth in fluctuating environments can be predicted quantitatively based on TPCs generated in constant laboratory conditions. With experimental populations of the green alga Tetraselmis tetrahele, we show that nonlinear averaging techniques accurately predicted increased as well as decreased population growth rates in fluctuating thermal regimes relative to constant thermal regimes. We extrapolate from these results to project critical temperatures for population growth and persistence of 89 phytoplankton species in naturally variable thermal environments. These results advance our ability to predict population dynamics in the context of global change.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check supplementary info, constant vs flux </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fig s6 </t>
   </si>
 </sst>
 </file>
@@ -861,8 +885,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -1180,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDF54A4-7244-6B4F-B3C6-F723070AAEF8}">
-  <dimension ref="A1:T35"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1925,770 +1950,814 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="2">
         <v>2012</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="1" t="s">
+      <c r="H17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="M17" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="O17" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:20" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="2">
         <v>2019</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="1" t="s">
+      <c r="H18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="M18" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:20" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="2">
         <v>2008</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="1" t="s">
+      <c r="H19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1" t="s">
+      <c r="L19" s="2"/>
+      <c r="M19" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1" t="s">
+      <c r="N19" s="2"/>
+      <c r="O19" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-    </row>
-    <row r="20" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+    </row>
+    <row r="20" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="2">
         <v>2017</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="1" t="s">
+      <c r="H20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="M20" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="O20" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="2">
         <v>2013</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="1" t="s">
+      <c r="H21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1" t="s">
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-    </row>
-    <row r="22" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+    </row>
+    <row r="22" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="2">
         <v>2015</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="1" t="s">
+      <c r="H22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="O22" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="2">
         <v>2010</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="1" t="s">
+      <c r="H23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1" t="s">
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-    </row>
-    <row r="24" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+    </row>
+    <row r="24" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="2">
         <v>2021</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="1" t="s">
+      <c r="H24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="O24" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="2">
         <v>2011</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="1" t="s">
+      <c r="H25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="M25" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="O25" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="2">
         <v>2020</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="1" t="s">
+      <c r="H26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="M26" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="O26" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="2">
         <v>2009</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="1" t="s">
+      <c r="H27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="O27" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:20" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="2">
         <v>2020</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="1" t="s">
+      <c r="H28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="O28" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="4">
         <v>2005</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J29" s="3" t="s">
+      <c r="H29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="M29" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="O29" s="3" t="s">
+      <c r="O29" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="4">
         <v>2019</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J30" s="3" t="s">
+      <c r="H30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="M30" s="3" t="s">
+      <c r="M30" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="O30" s="3" t="s">
+      <c r="O30" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="4">
         <v>2011</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="3" t="s">
+      <c r="H31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="M31" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="O31" s="3" t="s">
+      <c r="O31" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="4">
         <v>2016</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J32" s="3" t="s">
+      <c r="H32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="K32" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="M32" s="3" t="s">
+      <c r="M32" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="O32" s="3" t="s">
+      <c r="O32" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:16" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="4">
         <v>2018</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J33" s="3" t="s">
+      <c r="H33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="O33" s="3" t="s">
+      <c r="O33" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="4">
         <v>2020</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34" s="3" t="s">
+      <c r="H34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="K34" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="M34" s="3" t="s">
+      <c r="M34" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="O34" s="3" t="s">
+      <c r="O34" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="4">
         <v>2018</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J35" s="3" t="s">
+      <c r="H35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="M35" s="3" t="s">
+      <c r="M35" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="O35" s="3" t="s">
+      <c r="O35" s="4" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F36" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>